<commit_message>
allure package removed form pages
</commit_message>
<xml_diff>
--- a/target/test-classes/Excel/CloudPos.xlsx
+++ b/target/test-classes/Excel/CloudPos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IntelljWorkspaces\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535DA789-006E-4FEE-A579-001870413BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D726A8-90C3-4086-9522-5A3CA661E241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{411B86E3-5BC8-4162-9D5B-60D77C5E31A0}"/>
   </bookViews>
@@ -1975,7 +1975,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2258,7 +2258,7 @@
         <v>88</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>89</v>

</xml_diff>